<commit_message>
adding sprint 1 artificats and system architecture
</commit_message>
<xml_diff>
--- a/Documentation/Requirement Stacks.xlsx
+++ b/Documentation/Requirement Stacks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sabeenahmad/School/SeniorYear/Fall/EECS581/EECS581-Project3/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0A02B0-73F2-8540-BE8F-60DC3B4952CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7AC8C2D-DD41-864A-B00F-BBD838858D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{887C07AF-CBEC-C94A-80A8-993BC205310E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Requirment ID</t>
   </si>
@@ -83,15 +83,6 @@
     <t>Mark parking lots available to red permit holders.</t>
   </si>
   <si>
-    <t>Mark parking lots available to Mississippi Garage Holders</t>
-  </si>
-  <si>
-    <t>Mark parking lots available toUnion Garage holders.</t>
-  </si>
-  <si>
-    <t>Mark parking lots available to Green permit olders</t>
-  </si>
-  <si>
     <t>Provide a calendar view showing dates and times when parking is restricted due to campus events(e.g. Basektball Game)</t>
   </si>
   <si>
@@ -129,6 +120,12 @@
   </si>
   <si>
     <t>Add a filter that filters based on availability, permit, and distance</t>
+  </si>
+  <si>
+    <t>Mark parking lots available to Union Garage holders.</t>
+  </si>
+  <si>
+    <t>Mark parking lots available to Central District Parking Garage Holders</t>
   </si>
 </sst>
 </file>
@@ -508,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F1172D-E90C-514C-9649-9DE0EA96533A}">
-  <dimension ref="B2:F24"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,6 +590,9 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7">
@@ -621,6 +621,9 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9">
@@ -635,19 +638,25 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>4.3</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
@@ -655,7 +664,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -663,30 +672,33 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13">
         <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -694,10 +706,10 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -708,141 +720,130 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15">
-        <v>7</v>
+        <v>8.1</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>21</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
         <v>23</v>
       </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20">
         <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>26</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
         <v>25</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24">
-        <v>3</v>
-      </c>
-      <c r="E24" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>